<commit_message>
feat: minimal updates 2
nagmeeting kanina
</commit_message>
<xml_diff>
--- a/notebook-tests/EDA/UP Data Science Society AY2324A/Inte Internship.xlsx
+++ b/notebook-tests/EDA/UP Data Science Society AY2324A/Inte Internship.xlsx
@@ -789,7 +789,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,8 +802,23 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,8 +843,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -852,9 +877,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -865,16 +907,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1175,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1245,7 @@
     <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1251,59 +1295,59 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="J2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="5" t="str">
+      <c r="P2" s="4" t="str">
         <f>CONCATENATE(C2," ",B2)</f>
         <v>Achilles Sebastian Muyco</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>176</v>
       </c>
       <c r="B3" t="s">
@@ -1354,7 +1398,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
@@ -1404,7 +1448,7 @@
         <v>Cecillia Marie Carullo</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
@@ -1455,8 +1499,8 @@
         <v>Carl Miranda</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>185</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1506,8 +1550,8 @@
         <v>Daryl Lara</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:16" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1557,8 +1601,8 @@
         <v>Edgar Allan Mendoza</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B8" t="s">
@@ -1608,8 +1652,8 @@
         <v>Esteban Ii Ero</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>201</v>
       </c>
       <c r="B9" t="s">
@@ -1659,8 +1703,8 @@
         <v>Gian Carlo Torres</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B10" t="s">
@@ -1708,7 +1752,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>239</v>
       </c>
       <c r="B11" t="s">
@@ -1807,7 +1851,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B13" t="s">
@@ -1857,158 +1901,158 @@
         <v>Joshua Zachary Tappul</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:16" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="5" t="s">
+      <c r="J14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="5" t="str">
+      <c r="P14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Jess Vincent Ybut</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:16" s="4" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="I15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="5" t="s">
+      <c r="L15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="5" t="str">
+      <c r="P15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Mac Quay Labasano</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="5" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>171599873</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" s="7" t="s">
+      <c r="J16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="O16" s="7" t="s">
+      <c r="O16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="7" t="str">
+      <c r="P16" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Fender Ignacio</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>230</v>
       </c>
       <c r="B17" t="s">
@@ -2055,8 +2099,8 @@
         <v>Lian John Tiu</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B18" t="s">
@@ -2106,56 +2150,56 @@
         <v>Marife Zacarias</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" s="5" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" s="7" t="s">
+      <c r="J19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="P19" s="7" t="str">
+      <c r="P19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Roselle Mae Menchavez</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>167</v>
       </c>
       <c r="B20" t="s">
@@ -2205,8 +2249,8 @@
         <v>Morganne Gayle Lim</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B21" t="s">
@@ -2253,8 +2297,8 @@
         <v>Mike James Villanueva</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
@@ -2304,8 +2348,8 @@
         <v>Mark Jeffrey Zapanta</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B23" t="s">
@@ -2355,8 +2399,8 @@
         <v>Neil Awit</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>159</v>
       </c>
       <c r="B24" t="s">
@@ -2406,8 +2450,8 @@
         <v>Rodney James Iracta</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>153</v>
       </c>
       <c r="B25" t="s">
@@ -2454,8 +2498,8 @@
         <v>Rhyz Jover</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B26" t="s">
@@ -2505,7 +2549,7 @@
         <v>Raissa Chloe Curray</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>209</v>
       </c>
@@ -2556,8 +2600,8 @@
         <v>Regina Carla Bayongan</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B28" t="s">
@@ -2607,7 +2651,7 @@
         <v>Rosa Lea Baldevarona</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>193</v>
       </c>
@@ -2658,8 +2702,8 @@
         <v>Shanjid Abduhalim</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B30" t="s">
@@ -2709,10 +2753,12 @@
         <v>Steven Kyle Villanueva</v>
       </c>
     </row>
+    <row r="31" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sortState ref="A2:P32">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>